<commit_message>
- DS GDV: add {BuTruTraHang}
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Teamplate_GoiDichVu.xlsx
+++ b/banhang24/Template/ExportExcel/Teamplate_GoiDichVu.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Tên khách hàng</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Người tạo</t>
   </si>
   <si>
-    <t>Còn lại</t>
-  </si>
-  <si>
     <t>Tiền mặt</t>
   </si>
   <si>
@@ -107,6 +104,15 @@
   </si>
   <si>
     <t>Khách đã trả</t>
+  </si>
+  <si>
+    <t>Bù trừ trả hàng</t>
+  </si>
+  <si>
+    <t>Giá trị sau trả</t>
+  </si>
+  <si>
+    <t>Còn nợ</t>
   </si>
 </sst>
 </file>
@@ -650,12 +656,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA33"/>
+  <dimension ref="A1:AC33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,14 +678,14 @@
     <col min="14" max="15" width="18" style="28" customWidth="1"/>
     <col min="16" max="16" width="21" style="28" customWidth="1"/>
     <col min="17" max="17" width="19.140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="19.140625" style="28" customWidth="1"/>
-    <col min="24" max="24" width="18.140625" style="28" customWidth="1"/>
-    <col min="25" max="25" width="18.140625" style="7" customWidth="1"/>
-    <col min="26" max="26" width="21.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="9.140625" style="1"/>
+    <col min="18" max="25" width="19.140625" style="28" customWidth="1"/>
+    <col min="26" max="26" width="18.140625" style="28" customWidth="1"/>
+    <col min="27" max="27" width="18.140625" style="7" customWidth="1"/>
+    <col min="28" max="28" width="21.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>17</v>
       </c>
@@ -708,9 +714,11 @@
       <c r="X1" s="33"/>
       <c r="Y1" s="33"/>
       <c r="Z1" s="33"/>
-      <c r="AA1" s="5"/>
-    </row>
-    <row r="2" spans="1:27" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="5"/>
+    </row>
+    <row r="2" spans="1:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="22"/>
@@ -735,11 +743,13 @@
       <c r="V2" s="27"/>
       <c r="W2" s="27"/>
       <c r="X2" s="27"/>
-      <c r="Y2" s="25"/>
-      <c r="Z2" s="18"/>
-      <c r="AA2" s="5"/>
-    </row>
-    <row r="3" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="25"/>
+      <c r="AB2" s="18"/>
+      <c r="AC2" s="5"/>
+    </row>
+    <row r="3" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>13</v>
       </c>
@@ -766,11 +776,13 @@
       <c r="V3" s="27"/>
       <c r="W3" s="27"/>
       <c r="X3" s="27"/>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="18"/>
-      <c r="AA3" s="5"/>
-    </row>
-    <row r="4" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y3" s="27"/>
+      <c r="Z3" s="27"/>
+      <c r="AA3" s="25"/>
+      <c r="AB3" s="18"/>
+      <c r="AC3" s="5"/>
+    </row>
+    <row r="4" spans="1:29" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>14</v>
       </c>
@@ -796,12 +808,14 @@
       <c r="V4" s="27"/>
       <c r="W4" s="27"/>
       <c r="X4" s="27"/>
-      <c r="Y4" s="25"/>
-      <c r="Z4" s="18"/>
-      <c r="AA4" s="5"/>
-    </row>
-    <row r="5" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:27" s="8" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Y4" s="27"/>
+      <c r="Z4" s="27"/>
+      <c r="AA4" s="25"/>
+      <c r="AB4" s="18"/>
+      <c r="AC4" s="5"/>
+    </row>
+    <row r="5" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:29" s="8" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -815,10 +829,10 @@
         <v>16</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>0</v>
@@ -830,7 +844,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K6" s="10" t="s">
         <v>5</v>
@@ -845,7 +859,7 @@
         <v>8</v>
       </c>
       <c r="O6" s="29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P6" s="29" t="s">
         <v>9</v>
@@ -857,31 +871,37 @@
         <v>29</v>
       </c>
       <c r="S6" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="T6" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="U6" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="V6" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="T6" s="29" t="s">
+      <c r="W6" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="U6" s="29" t="s">
+      <c r="X6" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y6" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="V6" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="W6" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="X6" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y6" s="4" t="s">
+      <c r="Z6" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="Z6" s="10" t="s">
+      <c r="AB6" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="17"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
@@ -906,10 +926,12 @@
       <c r="V7" s="30"/>
       <c r="W7" s="30"/>
       <c r="X7" s="30"/>
-      <c r="Y7" s="6"/>
-      <c r="Z7" s="13"/>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Y7" s="30"/>
+      <c r="Z7" s="30"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="13"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
@@ -934,10 +956,12 @@
       <c r="V8" s="30"/>
       <c r="W8" s="30"/>
       <c r="X8" s="30"/>
-      <c r="Y8" s="6"/>
-      <c r="Z8" s="13"/>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Y8" s="30"/>
+      <c r="Z8" s="30"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="13"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
@@ -962,10 +986,12 @@
       <c r="V9" s="30"/>
       <c r="W9" s="30"/>
       <c r="X9" s="30"/>
-      <c r="Y9" s="6"/>
-      <c r="Z9" s="13"/>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Y9" s="30"/>
+      <c r="Z9" s="30"/>
+      <c r="AA9" s="6"/>
+      <c r="AB9" s="13"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
@@ -990,10 +1016,12 @@
       <c r="V10" s="30"/>
       <c r="W10" s="30"/>
       <c r="X10" s="30"/>
-      <c r="Y10" s="6"/>
-      <c r="Z10" s="13"/>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Y10" s="30"/>
+      <c r="Z10" s="30"/>
+      <c r="AA10" s="6"/>
+      <c r="AB10" s="13"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -1018,10 +1046,12 @@
       <c r="V11" s="30"/>
       <c r="W11" s="30"/>
       <c r="X11" s="30"/>
-      <c r="Y11" s="6"/>
-      <c r="Z11" s="13"/>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Y11" s="30"/>
+      <c r="Z11" s="30"/>
+      <c r="AA11" s="6"/>
+      <c r="AB11" s="13"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -1046,10 +1076,12 @@
       <c r="V12" s="30"/>
       <c r="W12" s="30"/>
       <c r="X12" s="30"/>
-      <c r="Y12" s="6"/>
-      <c r="Z12" s="13"/>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Y12" s="30"/>
+      <c r="Z12" s="30"/>
+      <c r="AA12" s="6"/>
+      <c r="AB12" s="13"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="17"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -1074,10 +1106,12 @@
       <c r="V13" s="30"/>
       <c r="W13" s="30"/>
       <c r="X13" s="30"/>
-      <c r="Y13" s="6"/>
-      <c r="Z13" s="13"/>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Y13" s="30"/>
+      <c r="Z13" s="30"/>
+      <c r="AA13" s="6"/>
+      <c r="AB13" s="13"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
@@ -1102,10 +1136,12 @@
       <c r="V14" s="30"/>
       <c r="W14" s="30"/>
       <c r="X14" s="30"/>
-      <c r="Y14" s="6"/>
-      <c r="Z14" s="13"/>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Y14" s="30"/>
+      <c r="Z14" s="30"/>
+      <c r="AA14" s="6"/>
+      <c r="AB14" s="13"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
@@ -1130,10 +1166,12 @@
       <c r="V15" s="30"/>
       <c r="W15" s="30"/>
       <c r="X15" s="30"/>
-      <c r="Y15" s="6"/>
-      <c r="Z15" s="13"/>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Y15" s="30"/>
+      <c r="Z15" s="30"/>
+      <c r="AA15" s="6"/>
+      <c r="AB15" s="13"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -1158,10 +1196,12 @@
       <c r="V16" s="30"/>
       <c r="W16" s="30"/>
       <c r="X16" s="30"/>
-      <c r="Y16" s="6"/>
-      <c r="Z16" s="13"/>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y16" s="30"/>
+      <c r="Z16" s="30"/>
+      <c r="AA16" s="6"/>
+      <c r="AB16" s="13"/>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -1186,10 +1226,12 @@
       <c r="V17" s="30"/>
       <c r="W17" s="30"/>
       <c r="X17" s="30"/>
-      <c r="Y17" s="6"/>
-      <c r="Z17" s="13"/>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y17" s="30"/>
+      <c r="Z17" s="30"/>
+      <c r="AA17" s="6"/>
+      <c r="AB17" s="13"/>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -1214,10 +1256,12 @@
       <c r="V18" s="30"/>
       <c r="W18" s="30"/>
       <c r="X18" s="30"/>
-      <c r="Y18" s="6"/>
-      <c r="Z18" s="13"/>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y18" s="30"/>
+      <c r="Z18" s="30"/>
+      <c r="AA18" s="6"/>
+      <c r="AB18" s="13"/>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -1242,10 +1286,12 @@
       <c r="V19" s="30"/>
       <c r="W19" s="30"/>
       <c r="X19" s="30"/>
-      <c r="Y19" s="6"/>
-      <c r="Z19" s="13"/>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y19" s="30"/>
+      <c r="Z19" s="30"/>
+      <c r="AA19" s="6"/>
+      <c r="AB19" s="13"/>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
@@ -1270,10 +1316,12 @@
       <c r="V20" s="30"/>
       <c r="W20" s="30"/>
       <c r="X20" s="30"/>
-      <c r="Y20" s="6"/>
-      <c r="Z20" s="13"/>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y20" s="30"/>
+      <c r="Z20" s="30"/>
+      <c r="AA20" s="6"/>
+      <c r="AB20" s="13"/>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -1298,10 +1346,12 @@
       <c r="V21" s="30"/>
       <c r="W21" s="30"/>
       <c r="X21" s="30"/>
-      <c r="Y21" s="6"/>
-      <c r="Z21" s="13"/>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y21" s="30"/>
+      <c r="Z21" s="30"/>
+      <c r="AA21" s="6"/>
+      <c r="AB21" s="13"/>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
@@ -1326,10 +1376,12 @@
       <c r="V22" s="30"/>
       <c r="W22" s="30"/>
       <c r="X22" s="30"/>
-      <c r="Y22" s="6"/>
-      <c r="Z22" s="13"/>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y22" s="30"/>
+      <c r="Z22" s="30"/>
+      <c r="AA22" s="6"/>
+      <c r="AB22" s="13"/>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="17"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
@@ -1354,10 +1406,12 @@
       <c r="V23" s="30"/>
       <c r="W23" s="30"/>
       <c r="X23" s="30"/>
-      <c r="Y23" s="6"/>
-      <c r="Z23" s="13"/>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y23" s="30"/>
+      <c r="Z23" s="30"/>
+      <c r="AA23" s="6"/>
+      <c r="AB23" s="13"/>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
@@ -1382,10 +1436,12 @@
       <c r="V24" s="30"/>
       <c r="W24" s="30"/>
       <c r="X24" s="30"/>
-      <c r="Y24" s="6"/>
-      <c r="Z24" s="13"/>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y24" s="30"/>
+      <c r="Z24" s="30"/>
+      <c r="AA24" s="6"/>
+      <c r="AB24" s="13"/>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="17"/>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
@@ -1410,10 +1466,12 @@
       <c r="V25" s="30"/>
       <c r="W25" s="30"/>
       <c r="X25" s="30"/>
-      <c r="Y25" s="6"/>
-      <c r="Z25" s="13"/>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y25" s="30"/>
+      <c r="Z25" s="30"/>
+      <c r="AA25" s="6"/>
+      <c r="AB25" s="13"/>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
@@ -1438,10 +1496,12 @@
       <c r="V26" s="30"/>
       <c r="W26" s="30"/>
       <c r="X26" s="30"/>
-      <c r="Y26" s="6"/>
-      <c r="Z26" s="13"/>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y26" s="30"/>
+      <c r="Z26" s="30"/>
+      <c r="AA26" s="6"/>
+      <c r="AB26" s="13"/>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
@@ -1466,10 +1526,12 @@
       <c r="V27" s="30"/>
       <c r="W27" s="30"/>
       <c r="X27" s="30"/>
-      <c r="Y27" s="6"/>
-      <c r="Z27" s="13"/>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y27" s="30"/>
+      <c r="Z27" s="30"/>
+      <c r="AA27" s="6"/>
+      <c r="AB27" s="13"/>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -1494,10 +1556,12 @@
       <c r="V28" s="30"/>
       <c r="W28" s="30"/>
       <c r="X28" s="30"/>
-      <c r="Y28" s="6"/>
-      <c r="Z28" s="13"/>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y28" s="30"/>
+      <c r="Z28" s="30"/>
+      <c r="AA28" s="6"/>
+      <c r="AB28" s="13"/>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="16"/>
       <c r="C29" s="16"/>
@@ -1522,10 +1586,12 @@
       <c r="V29" s="30"/>
       <c r="W29" s="30"/>
       <c r="X29" s="30"/>
-      <c r="Y29" s="6"/>
-      <c r="Z29" s="13"/>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y29" s="30"/>
+      <c r="Z29" s="30"/>
+      <c r="AA29" s="6"/>
+      <c r="AB29" s="13"/>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
@@ -1550,10 +1616,12 @@
       <c r="V30" s="30"/>
       <c r="W30" s="30"/>
       <c r="X30" s="30"/>
-      <c r="Y30" s="6"/>
-      <c r="Z30" s="13"/>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y30" s="30"/>
+      <c r="Z30" s="30"/>
+      <c r="AA30" s="6"/>
+      <c r="AB30" s="13"/>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" s="34" t="s">
         <v>12</v>
       </c>
@@ -1613,10 +1681,18 @@
         <f>SUM(X$7:X30)</f>
         <v>0</v>
       </c>
-      <c r="Y31" s="20"/>
-      <c r="Z31" s="19"/>
-    </row>
-    <row r="33" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="Y31" s="31">
+        <f>SUM(Y$7:Y30)</f>
+        <v>0</v>
+      </c>
+      <c r="Z31" s="31">
+        <f>SUM(Z$7:Z30)</f>
+        <v>0</v>
+      </c>
+      <c r="AA31" s="20"/>
+      <c r="AB31" s="19"/>
+    </row>
+    <row r="33" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -1640,12 +1716,14 @@
       <c r="V33" s="32"/>
       <c r="W33" s="32"/>
       <c r="X33" s="32"/>
-      <c r="Y33" s="1"/>
-      <c r="Z33" s="1"/>
+      <c r="Y33" s="32"/>
+      <c r="Z33" s="32"/>
+      <c r="AA33" s="1"/>
+      <c r="AB33" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:Z1"/>
+    <mergeCell ref="A1:AB1"/>
     <mergeCell ref="A31:M31"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>

</xml_diff>